<commit_message>
"convert xlsx to csv for embedding"
</commit_message>
<xml_diff>
--- a/nodejs/data/Menu_drinks2.xlsx
+++ b/nodejs/data/Menu_drinks2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ddca7f07d79f143e/Desktop/cohort28/c28-bad-proj-07-sw/nodejs/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethdouglasslai/teckyC28/c28-bad-proj-07-sw/nodejs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{732F8B38-C486-4A26-9B2B-576B4F79899C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FEA4553-C610-4E72-8906-C74A200853A3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416236F2-1952-CE4D-BFE7-07CB1624F5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="14055" yWindow="-18885" windowWidth="19275" windowHeight="16695" xr2:uid="{9E7474C8-1A9C-4E5B-9CAA-AE29F6E4FFE7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19860" xr2:uid="{9E7474C8-1A9C-4E5B-9CAA-AE29F6E4FFE7}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -535,15 +535,15 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -569,7 +569,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -581,7 +581,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -593,7 +593,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -605,7 +605,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -617,7 +617,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -629,7 +629,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -641,7 +641,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -653,7 +653,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -665,7 +665,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -677,7 +677,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -689,7 +689,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -701,7 +701,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -713,7 +713,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -725,7 +725,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -737,7 +737,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -749,7 +749,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -761,7 +761,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -773,7 +773,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -785,7 +785,7 @@
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
@@ -797,7 +797,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -809,7 +809,7 @@
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -821,7 +821,7 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
@@ -833,7 +833,7 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -845,7 +845,7 @@
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
@@ -857,7 +857,7 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -869,7 +869,7 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>